<commit_message>
data: removed empty lines
</commit_message>
<xml_diff>
--- a/data/db-preload.xlsx
+++ b/data/db-preload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduard\repos\FitnessTracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF272A8-546C-42AE-B237-30D65C7273A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E018A89-33F7-4EA7-9C92-A272405904AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="18600" activeTab="1" xr2:uid="{D5405B73-0EDF-478A-9825-0B462EFB9FF2}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{D5405B73-0EDF-478A-9825-0B462EFB9FF2}"/>
   </bookViews>
   <sheets>
     <sheet name="muscles" sheetId="1" r:id="rId1"/>
@@ -653,74 +653,74 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -733,22 +733,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BBAA8C7-91E4-4F37-B3F4-0B177CCBE0B5}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -765,7 +765,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -779,7 +779,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -793,7 +793,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -807,7 +807,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -821,7 +821,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -835,7 +835,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -849,7 +849,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -863,7 +863,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -877,7 +877,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -891,148 +891,218 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
       <c r="E13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
       <c r="E14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
-        <v>70</v>
-      </c>
       <c r="E20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1041,303 +1111,233 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>86</v>
       </c>
       <c r="E42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="E45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" t="s">
-        <v>86</v>
-      </c>
-      <c r="E52" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" t="s">
-        <v>12</v>
-      </c>
-      <c r="D57" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" t="s">
-        <v>89</v>
-      </c>
-      <c r="E59" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>